<commit_message>
food enviroment variables added to the urban dicts
</commit_message>
<xml_diff>
--- a/dictionaries/urban_ath/1_3/1_3_trimester_rep.xlsx
+++ b/dictionaries/urban_ath/1_3/1_3_trimester_rep.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\PROJECTS\ATHLETE\DOCUMENTS\dictionaries\jose_dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="13_ncr:1_{461D9A8A-77D4-4490-A83E-82B1CB5F75F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9A194FE-4586-4C81-9660-BBDBE9C70514}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F9EC3B-C949-41BD-AEE5-4758A5926631}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32760" yWindow="32760" windowWidth="16380" windowHeight="8190" tabRatio="256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,23 +17,12 @@
     <sheet name="Categories" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Variables!$A$1:$D$126</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -45,7 +34,7 @@
     <author>JOSÉ MIGUEL, URQUIZA ORTIZ</author>
   </authors>
   <commentList>
-    <comment ref="C103" authorId="0" shapeId="0" xr:uid="{167633DA-362C-4BEF-A089-209DC6C3E00C}">
+    <comment ref="C125" authorId="0" shapeId="0" xr:uid="{167633DA-362C-4BEF-A089-209DC6C3E00C}">
       <text>
         <r>
           <rPr>
@@ -74,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="351">
   <si>
     <t>name</t>
   </si>
@@ -995,13 +984,145 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>ath_fefoodenv300_t</t>
+  </si>
+  <si>
+    <t>ath_fealcohol300_t</t>
+  </si>
+  <si>
+    <t>ath_febar300_t</t>
+  </si>
+  <si>
+    <t>ath_febeverages300_t</t>
+  </si>
+  <si>
+    <t>ath_febiergarten300_t</t>
+  </si>
+  <si>
+    <t>ath_fecafe300_t</t>
+  </si>
+  <si>
+    <t>ath_feconvenience300_t</t>
+  </si>
+  <si>
+    <t>ath_fefastfood300_t</t>
+  </si>
+  <si>
+    <t>ath_fepub300_t</t>
+  </si>
+  <si>
+    <t>ath_ferestaurant300_t</t>
+  </si>
+  <si>
+    <t>ath_fesupermarket300_t</t>
+  </si>
+  <si>
+    <t>ath_fefoodenv800_t</t>
+  </si>
+  <si>
+    <t>ath_fealcohol800_t</t>
+  </si>
+  <si>
+    <t>ath_febar800_t</t>
+  </si>
+  <si>
+    <t>ath_febeverages800_t</t>
+  </si>
+  <si>
+    <t>ath_febiergarten800_t</t>
+  </si>
+  <si>
+    <t>ath_fecafe800_t</t>
+  </si>
+  <si>
+    <t>ath_feconvenience800_t</t>
+  </si>
+  <si>
+    <t>ath_fefastfood800_t</t>
+  </si>
+  <si>
+    <t>ath_fepub800_t</t>
+  </si>
+  <si>
+    <t>ath_ferestaurant800_t</t>
+  </si>
+  <si>
+    <t>ath_fesupermarket800_t</t>
+  </si>
+  <si>
+    <t>number of facilities related to food divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to alcohol establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to bar establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to beverages establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to biergarten establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to cafe establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to convenience establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to fast food establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to pub establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to restaurant establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to supermarket establishments divided by the area of the 300 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to food divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to alcohol establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to bar establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to beverages establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to biergarten establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to cafe establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to convenience establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to fast food establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to pub establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to restaurant establishments divided by the area of the 800 meters buffer at trimester</t>
+  </si>
+  <si>
+    <t>number of facilities related to supermarket establishments divided by the area of the 800 meters buffer at trimester</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="26">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1968,20 +2089,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="26" style="1" customWidth="1"/>
     <col min="5" max="16384" width="10.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1995,7 +2114,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" customFormat="1">
+    <row r="2" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2009,7 +2128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" customFormat="1">
+    <row r="3" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2020,7 +2139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" customFormat="1">
+    <row r="4" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2031,7 +2150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="6" customFormat="1">
+    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -2045,7 +2164,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" customFormat="1">
+    <row r="6" spans="1:4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2059,7 +2178,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:4" customFormat="1" ht="14.25" customHeight="1">
+    <row r="7" spans="1:4" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -2070,7 +2189,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -2084,7 +2203,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2098,7 +2217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -2112,7 +2231,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -2126,7 +2245,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -2140,7 +2259,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -2154,7 +2273,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2168,7 +2287,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2182,7 +2301,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2196,7 +2315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -2210,7 +2329,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>43</v>
       </c>
@@ -2224,7 +2343,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>45</v>
       </c>
@@ -2238,7 +2357,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -2252,7 +2371,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -2266,7 +2385,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>51</v>
       </c>
@@ -2280,7 +2399,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -2294,7 +2413,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>55</v>
       </c>
@@ -2308,7 +2427,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -2322,7 +2441,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>59</v>
       </c>
@@ -2336,7 +2455,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -2350,7 +2469,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -2364,7 +2483,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -2378,7 +2497,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -2392,7 +2511,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>69</v>
       </c>
@@ -2406,7 +2525,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -2420,7 +2539,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -2434,7 +2553,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>76</v>
       </c>
@@ -2448,7 +2567,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -2462,7 +2581,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="12" customFormat="1">
+    <row r="36" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>81</v>
       </c>
@@ -2474,7 +2593,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="12" customFormat="1">
+    <row r="37" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>83</v>
       </c>
@@ -2486,7 +2605,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>85</v>
       </c>
@@ -2500,7 +2619,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -2514,7 +2633,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>90</v>
       </c>
@@ -2528,7 +2647,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2542,7 +2661,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>94</v>
       </c>
@@ -2556,7 +2675,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2570,7 +2689,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -2584,7 +2703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>101</v>
       </c>
@@ -2598,7 +2717,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>103</v>
       </c>
@@ -2612,7 +2731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>105</v>
       </c>
@@ -2626,7 +2745,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>108</v>
       </c>
@@ -2640,7 +2759,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>111</v>
       </c>
@@ -2654,7 +2773,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>113</v>
       </c>
@@ -2668,7 +2787,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>116</v>
       </c>
@@ -2682,7 +2801,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>118</v>
       </c>
@@ -2696,7 +2815,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>121</v>
       </c>
@@ -2710,7 +2829,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>123</v>
       </c>
@@ -2724,7 +2843,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>125</v>
       </c>
@@ -2738,7 +2857,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>127</v>
       </c>
@@ -2752,7 +2871,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>129</v>
       </c>
@@ -2766,7 +2885,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>131</v>
       </c>
@@ -2780,7 +2899,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>133</v>
       </c>
@@ -2792,7 +2911,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>135</v>
       </c>
@@ -2804,7 +2923,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>137</v>
       </c>
@@ -2816,7 +2935,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>139</v>
       </c>
@@ -2830,7 +2949,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>141</v>
       </c>
@@ -2844,7 +2963,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>143</v>
       </c>
@@ -2858,7 +2977,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>145</v>
       </c>
@@ -2872,7 +2991,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>147</v>
       </c>
@@ -2886,7 +3005,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -2900,7 +3019,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>151</v>
       </c>
@@ -2914,7 +3033,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>153</v>
       </c>
@@ -2928,7 +3047,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>155</v>
       </c>
@@ -2942,7 +3061,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>157</v>
       </c>
@@ -2956,7 +3075,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>159</v>
       </c>
@@ -2970,7 +3089,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>161</v>
       </c>
@@ -2984,7 +3103,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>163</v>
       </c>
@@ -2996,7 +3115,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>165</v>
       </c>
@@ -3008,7 +3127,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>167</v>
       </c>
@@ -3022,7 +3141,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>170</v>
       </c>
@@ -3036,7 +3155,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>173</v>
       </c>
@@ -3050,7 +3169,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -3064,7 +3183,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>178</v>
       </c>
@@ -3078,7 +3197,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>181</v>
       </c>
@@ -3092,7 +3211,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>183</v>
       </c>
@@ -3104,7 +3223,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>185</v>
       </c>
@@ -3116,7 +3235,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>187</v>
       </c>
@@ -3130,7 +3249,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>189</v>
       </c>
@@ -3144,280 +3263,588 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>307</v>
+      </c>
+      <c r="B86" t="s">
+        <v>20</v>
+      </c>
+      <c r="C86" t="s">
+        <v>114</v>
+      </c>
+      <c r="D86" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>308</v>
+      </c>
+      <c r="B87" t="s">
+        <v>20</v>
+      </c>
+      <c r="C87" t="s">
+        <v>114</v>
+      </c>
+      <c r="D87" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>309</v>
+      </c>
+      <c r="B88" t="s">
+        <v>20</v>
+      </c>
+      <c r="C88" t="s">
+        <v>114</v>
+      </c>
+      <c r="D88" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>310</v>
+      </c>
+      <c r="B89" t="s">
+        <v>20</v>
+      </c>
+      <c r="C89" t="s">
+        <v>114</v>
+      </c>
+      <c r="D89" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>311</v>
+      </c>
+      <c r="B90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C90" t="s">
+        <v>114</v>
+      </c>
+      <c r="D90" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>312</v>
+      </c>
+      <c r="B91" t="s">
+        <v>20</v>
+      </c>
+      <c r="C91" t="s">
+        <v>114</v>
+      </c>
+      <c r="D91" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>313</v>
+      </c>
+      <c r="B92" t="s">
+        <v>20</v>
+      </c>
+      <c r="C92" t="s">
+        <v>114</v>
+      </c>
+      <c r="D92" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>314</v>
+      </c>
+      <c r="B93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C93" t="s">
+        <v>114</v>
+      </c>
+      <c r="D93" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>315</v>
+      </c>
+      <c r="B94" t="s">
+        <v>20</v>
+      </c>
+      <c r="C94" t="s">
+        <v>114</v>
+      </c>
+      <c r="D94" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>316</v>
+      </c>
+      <c r="B95" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" t="s">
+        <v>114</v>
+      </c>
+      <c r="D95" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>317</v>
+      </c>
+      <c r="B96" t="s">
+        <v>20</v>
+      </c>
+      <c r="C96" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>318</v>
+      </c>
+      <c r="B97" t="s">
+        <v>20</v>
+      </c>
+      <c r="C97" t="s">
+        <v>114</v>
+      </c>
+      <c r="D97" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>319</v>
+      </c>
+      <c r="B98" t="s">
+        <v>20</v>
+      </c>
+      <c r="C98" t="s">
+        <v>114</v>
+      </c>
+      <c r="D98" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>320</v>
+      </c>
+      <c r="B99" t="s">
+        <v>20</v>
+      </c>
+      <c r="C99" t="s">
+        <v>114</v>
+      </c>
+      <c r="D99" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>321</v>
+      </c>
+      <c r="B100" t="s">
+        <v>20</v>
+      </c>
+      <c r="C100" t="s">
+        <v>114</v>
+      </c>
+      <c r="D100" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>322</v>
+      </c>
+      <c r="B101" t="s">
+        <v>20</v>
+      </c>
+      <c r="C101" t="s">
+        <v>114</v>
+      </c>
+      <c r="D101" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>323</v>
+      </c>
+      <c r="B102" t="s">
+        <v>20</v>
+      </c>
+      <c r="C102" t="s">
+        <v>114</v>
+      </c>
+      <c r="D102" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>324</v>
+      </c>
+      <c r="B103" t="s">
+        <v>20</v>
+      </c>
+      <c r="C103" t="s">
+        <v>114</v>
+      </c>
+      <c r="D103" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>325</v>
+      </c>
+      <c r="B104" t="s">
+        <v>20</v>
+      </c>
+      <c r="C104" t="s">
+        <v>114</v>
+      </c>
+      <c r="D104" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>326</v>
+      </c>
+      <c r="B105" t="s">
+        <v>20</v>
+      </c>
+      <c r="C105" t="s">
+        <v>114</v>
+      </c>
+      <c r="D105" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>327</v>
+      </c>
+      <c r="B106" t="s">
+        <v>20</v>
+      </c>
+      <c r="C106" t="s">
+        <v>114</v>
+      </c>
+      <c r="D106" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>328</v>
+      </c>
+      <c r="B107" t="s">
+        <v>20</v>
+      </c>
+      <c r="C107" t="s">
+        <v>114</v>
+      </c>
+      <c r="D107" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>191</v>
       </c>
-      <c r="B86" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="B108" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C108" t="s">
         <v>192</v>
       </c>
-      <c r="D86" t="s">
+      <c r="D108" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
-      <c r="A87" t="s">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
         <v>194</v>
       </c>
-      <c r="B87" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="B109" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C109" t="s">
         <v>192</v>
       </c>
-      <c r="D87" t="s">
+      <c r="D109" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
-      <c r="A88" t="s">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
         <v>196</v>
       </c>
-      <c r="B88" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="B110" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C110" t="s">
         <v>192</v>
       </c>
-      <c r="D88" t="s">
+      <c r="D110" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
-      <c r="A89" t="s">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>198</v>
       </c>
-      <c r="B89" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="B111" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C111" t="s">
         <v>99</v>
       </c>
-      <c r="D89" t="s">
+      <c r="D111" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
-      <c r="A90" t="s">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
         <v>200</v>
       </c>
-      <c r="B90" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="B112" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C112" t="s">
         <v>99</v>
       </c>
-      <c r="D90" t="s">
+      <c r="D112" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
-      <c r="A91" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
         <v>202</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="B113" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C113" t="s">
         <v>99</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D113" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
-      <c r="A92" t="s">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
         <v>204</v>
       </c>
-      <c r="B92" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="B114" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C114" t="s">
         <v>192</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D114" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:4">
-      <c r="A93" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
         <v>206</v>
       </c>
-      <c r="B93" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="B115" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C115" t="s">
         <v>192</v>
       </c>
-      <c r="D93" t="s">
+      <c r="D115" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
-      <c r="A94" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>208</v>
       </c>
-      <c r="B94" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="B116" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C116" t="s">
         <v>192</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D116" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
-      <c r="A95" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
         <v>210</v>
       </c>
-      <c r="B95" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="B117" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C117" t="s">
         <v>99</v>
       </c>
-      <c r="D95" t="s">
+      <c r="D117" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
-      <c r="A96" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
         <v>212</v>
       </c>
-      <c r="B96" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C96" t="s">
+      <c r="B118" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C118" t="s">
         <v>213</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D118" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="97" spans="1:4">
-      <c r="A97" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
         <v>215</v>
       </c>
-      <c r="B97" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C97" t="s">
+      <c r="B119" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C119" t="s">
         <v>216</v>
       </c>
-      <c r="D97" t="s">
+      <c r="D119" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="98" spans="1:4">
-      <c r="A98" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
         <v>218</v>
       </c>
-      <c r="B98" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="B120" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C120" t="s">
         <v>219</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D120" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="99" spans="1:4">
-      <c r="A99" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
         <v>221</v>
       </c>
-      <c r="B99" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="B121" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C121" t="s">
         <v>222</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D121" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="100" spans="1:4">
-      <c r="A100" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
         <v>224</v>
       </c>
-      <c r="B100" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="B122" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C122" t="s">
         <v>222</v>
       </c>
-      <c r="D100" t="s">
+      <c r="D122" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="101" spans="1:4">
-      <c r="A101" t="s">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
         <v>226</v>
       </c>
-      <c r="B101" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="B123" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C123" t="s">
         <v>222</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D123" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="102" spans="1:4">
-      <c r="A102" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
         <v>228</v>
       </c>
-      <c r="B102" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="B124" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C124" t="s">
         <v>192</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D124" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="103" spans="1:4">
-      <c r="A103" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" t="s">
         <v>230</v>
       </c>
-      <c r="B103" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="B125" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C125" t="s">
         <v>72</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D125" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
-      <c r="A104" s="1" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C104" s="1" t="s">
+      <c r="B126" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C126" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="D104" s="1" t="s">
+      <c r="D126" s="1" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="105" spans="1:4">
-      <c r="C105"/>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C127"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <autoFilter ref="A1:D104" xr:uid="{2A8193EC-26C3-47E8-AA62-347275DAEFB0}"/>
+  <autoFilter ref="A1:D126" xr:uid="{2A8193EC-26C3-47E8-AA62-347275DAEFB0}"/>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" sqref="A14:A15 B7 B5 B36:B43" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" showErrorMessage="1" sqref="A14:A15 B7 B5 B36:B43 B86:B107" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"integer,decimal,text,binary,locale,boolean,datetime,date"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3437,13 +3864,13 @@
       <selection activeCell="D82" sqref="A2:D82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="26" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="15">
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>235</v>
       </c>
@@ -3457,7 +3884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
@@ -3471,7 +3898,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>13</v>
       </c>
@@ -3485,7 +3912,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -3499,7 +3926,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>13</v>
       </c>
@@ -3513,7 +3940,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>13</v>
       </c>
@@ -3527,7 +3954,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
@@ -3541,7 +3968,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>13</v>
       </c>
@@ -3555,7 +3982,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -3569,7 +3996,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>13</v>
       </c>
@@ -3583,7 +4010,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>13</v>
       </c>
@@ -3597,7 +4024,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>13</v>
       </c>
@@ -3611,7 +4038,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
@@ -3625,7 +4052,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
@@ -3639,7 +4066,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>13</v>
       </c>
@@ -3653,7 +4080,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>13</v>
       </c>
@@ -3667,7 +4094,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15">
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>13</v>
       </c>
@@ -3681,7 +4108,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>13</v>
       </c>
@@ -3695,7 +4122,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
@@ -3709,7 +4136,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>13</v>
       </c>
@@ -3723,7 +4150,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>13</v>
       </c>
@@ -3737,7 +4164,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15">
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>13</v>
       </c>
@@ -3751,7 +4178,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15">
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>13</v>
       </c>
@@ -3765,7 +4192,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15">
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>13</v>
       </c>
@@ -3779,7 +4206,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15">
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>13</v>
       </c>
@@ -3793,7 +4220,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>13</v>
       </c>
@@ -3807,7 +4234,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15">
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>13</v>
       </c>
@@ -3821,7 +4248,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>13</v>
       </c>
@@ -3835,7 +4262,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15">
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>13</v>
       </c>
@@ -3849,7 +4276,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>13</v>
       </c>
@@ -3863,7 +4290,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>13</v>
       </c>
@@ -3877,7 +4304,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15">
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>13</v>
       </c>
@@ -3891,7 +4318,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>13</v>
       </c>
@@ -3905,7 +4332,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>17</v>
       </c>
@@ -3919,7 +4346,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>17</v>
       </c>
@@ -3933,7 +4360,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>17</v>
       </c>
@@ -3947,7 +4374,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>17</v>
       </c>
@@ -3961,7 +4388,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="10" t="s">
         <v>17</v>
       </c>
@@ -3975,7 +4402,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="10" t="s">
         <v>17</v>
       </c>
@@ -3989,7 +4416,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>17</v>
       </c>
@@ -4003,7 +4430,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="10" t="s">
         <v>17</v>
       </c>
@@ -4017,7 +4444,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="10" t="s">
         <v>17</v>
       </c>
@@ -4031,7 +4458,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15">
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="10" t="s">
         <v>17</v>
       </c>
@@ -4045,7 +4472,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15">
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="10" t="s">
         <v>17</v>
       </c>
@@ -4059,7 +4486,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15">
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="10" t="s">
         <v>17</v>
       </c>
@@ -4073,7 +4500,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15">
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="10" t="s">
         <v>17</v>
       </c>
@@ -4087,7 +4514,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15">
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
         <v>17</v>
       </c>
@@ -4101,7 +4528,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15">
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="10" t="s">
         <v>17</v>
       </c>
@@ -4115,7 +4542,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15">
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="10" t="s">
         <v>17</v>
       </c>
@@ -4129,7 +4556,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15">
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="10" t="s">
         <v>17</v>
       </c>
@@ -4143,7 +4570,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15">
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="10" t="s">
         <v>17</v>
       </c>
@@ -4157,7 +4584,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15">
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="10" t="s">
         <v>17</v>
       </c>
@@ -4171,7 +4598,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15">
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="10" t="s">
         <v>17</v>
       </c>
@@ -4185,7 +4612,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15">
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="10" t="s">
         <v>17</v>
       </c>
@@ -4199,7 +4626,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15">
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="10" t="s">
         <v>17</v>
       </c>
@@ -4213,7 +4640,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15">
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="10" t="s">
         <v>17</v>
       </c>
@@ -4227,7 +4654,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15">
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
         <v>17</v>
       </c>
@@ -4241,7 +4668,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15">
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
         <v>17</v>
       </c>
@@ -4255,7 +4682,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15">
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>163</v>
       </c>
@@ -4269,7 +4696,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15">
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>163</v>
       </c>
@@ -4283,7 +4710,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15">
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>163</v>
       </c>
@@ -4297,7 +4724,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15">
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>165</v>
       </c>
@@ -4311,7 +4738,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15">
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>165</v>
       </c>
@@ -4325,7 +4752,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15">
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>165</v>
       </c>
@@ -4339,7 +4766,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15">
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="s">
         <v>165</v>
       </c>
@@ -4353,7 +4780,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15">
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>165</v>
       </c>
@@ -4367,7 +4794,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15">
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="s">
         <v>183</v>
       </c>
@@ -4381,7 +4808,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15">
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="s">
         <v>183</v>
       </c>
@@ -4395,7 +4822,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15">
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="s">
         <v>183</v>
       </c>
@@ -4409,7 +4836,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15">
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="s">
         <v>183</v>
       </c>
@@ -4423,7 +4850,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15">
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="s">
         <v>183</v>
       </c>
@@ -4437,7 +4864,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15">
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="s">
         <v>183</v>
       </c>
@@ -4451,7 +4878,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15">
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="s">
         <v>185</v>
       </c>
@@ -4465,7 +4892,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15">
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="s">
         <v>185</v>
       </c>
@@ -4479,7 +4906,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15">
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="s">
         <v>185</v>
       </c>
@@ -4493,7 +4920,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15">
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="s">
         <v>185</v>
       </c>
@@ -4507,7 +4934,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15">
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="s">
         <v>185</v>
       </c>
@@ -4521,7 +4948,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15">
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
         <v>185</v>
       </c>
@@ -4535,7 +4962,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15">
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
         <v>81</v>
       </c>
@@ -4549,7 +4976,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15">
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="s">
         <v>83</v>
       </c>
@@ -4563,7 +4990,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15">
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="s">
         <v>81</v>
       </c>
@@ -4577,7 +5004,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15">
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="s">
         <v>83</v>
       </c>

</xml_diff>